<commit_message>
add notification, fix config, fix tests
</commit_message>
<xml_diff>
--- a/resources/template-courses.xlsx
+++ b/resources/template-courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bohda\PycharmProjects\project_YEDA\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F7C6E5-A1D3-4F6C-B896-47E00D8FCCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDA275E-E1CB-44B3-8884-2913754147CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10452" yWindow="3348" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>city</t>
   </si>
@@ -90,21 +90,6 @@
     <t>Kharkiv</t>
   </si>
   <si>
-    <t>Jared_Moreno1@gmail.com</t>
-  </si>
-  <si>
-    <t>Rafael_Hopkins2@gmail.com</t>
-  </si>
-  <si>
-    <t>Manuel_Ross3@gmail.com</t>
-  </si>
-  <si>
-    <t>Roger_Hanson3@gmail.com</t>
-  </si>
-  <si>
-    <t>Richard_Nichols4@gmail.com</t>
-  </si>
-  <si>
     <t>Richard Nichol</t>
   </si>
   <si>
@@ -120,26 +105,29 @@
     <t>Jared Moren</t>
   </si>
   <si>
-    <t>Richard_Nichol</t>
-  </si>
-  <si>
-    <t>Roger_Hans</t>
-  </si>
-  <si>
-    <t>Manuel_Ro</t>
-  </si>
-  <si>
-    <t>Raf_Hopkins</t>
-  </si>
-  <si>
-    <t>Jared_Moren</t>
+    <t>Jared_Moreno100@gmail.com</t>
+  </si>
+  <si>
+    <t>Rafael_Hopkins112@gmail.com</t>
+  </si>
+  <si>
+    <t>Manuel_Ross301@gmail.com</t>
+  </si>
+  <si>
+    <t>Roger_Hanson366@gmail.com</t>
+  </si>
+  <si>
+    <t>Richard_Nichols452@gmail.com</t>
+  </si>
+  <si>
+    <t>birthdate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -160,6 +148,13 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -204,13 +199,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -427,141 +424,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="27" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>852991250</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>123475012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>810530341</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>203489001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>768069432</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>356203321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>725608523</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>999745147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>683147614</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
+      <c r="F6">
+        <v>357621000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>810530341</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>768069432</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>725608523</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>683147614</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1548,14 +1551,14 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{5345DBB3-B1AC-4151-A53C-95968B902A1E}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{400B0DB1-B4BA-44E1-9BEF-77ADD9312F18}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{4C02A4E0-2781-4CAA-8463-D1827A68D85F}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{52E8A008-8D3F-437D-98FB-090FA137BB4D}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{C7063AA7-7645-4F02-8CAC-5FFC8A395709}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5345DBB3-B1AC-4151-A53C-95968B902A1E}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{400B0DB1-B4BA-44E1-9BEF-77ADD9312F18}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{4C02A4E0-2781-4CAA-8463-D1827A68D85F}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{52E8A008-8D3F-437D-98FB-090FA137BB4D}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{C7063AA7-7645-4F02-8CAC-5FFC8A395709}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>